<commit_message>
scatterplot revisions to include country code labels and Access data only
</commit_message>
<xml_diff>
--- a/data/Access_elec_CO2.xlsx
+++ b/data/Access_elec_CO2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbess/Data_Viz/JBess_final_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbess/Data_Viz/JBess_final_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -170,9 +170,6 @@
     <t>CO2KWHd1_2016</t>
   </si>
   <si>
-    <t>iso</t>
-  </si>
-  <si>
     <t>AGO</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>ZMB</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -667,7 +667,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -693,7 +693,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -719,7 +719,7 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -771,7 +771,7 @@
         <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -797,7 +797,7 @@
         <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -823,7 +823,7 @@
         <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -849,7 +849,7 @@
         <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -875,7 +875,7 @@
         <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -901,7 +901,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -927,7 +927,7 @@
         <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -953,7 +953,7 @@
         <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -979,7 +979,7 @@
         <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1005,7 +1005,7 @@
         <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -1031,7 +1031,7 @@
         <v>266</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1057,7 +1057,7 @@
         <v>288</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1083,7 +1083,7 @@
         <v>320</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1109,7 +1109,7 @@
         <v>332</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
@@ -1135,7 +1135,7 @@
         <v>340</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -1161,7 +1161,7 @@
         <v>356</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -1187,7 +1187,7 @@
         <v>360</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
@@ -1213,7 +1213,7 @@
         <v>384</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>11</v>
@@ -1239,7 +1239,7 @@
         <v>388</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1265,7 +1265,7 @@
         <v>404</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
@@ -1291,7 +1291,7 @@
         <v>414</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
@@ -1317,7 +1317,7 @@
         <v>591</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>26</v>
@@ -1343,7 +1343,7 @@
         <v>604</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
@@ -1369,7 +1369,7 @@
         <v>608</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1395,7 +1395,7 @@
         <v>634</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>29</v>
@@ -1421,7 +1421,7 @@
         <v>682</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
@@ -1447,7 +1447,7 @@
         <v>686</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
@@ -1473,7 +1473,7 @@
         <v>710</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
@@ -1499,7 +1499,7 @@
         <v>716</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
         <v>40</v>
@@ -1525,7 +1525,7 @@
         <v>736</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -1551,7 +1551,7 @@
         <v>748</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
@@ -1577,7 +1577,7 @@
         <v>760</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
@@ -1603,7 +1603,7 @@
         <v>834</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1629,7 +1629,7 @@
         <v>887</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
@@ -1655,7 +1655,7 @@
         <v>894</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>

</xml_diff>